<commit_message>
luban调整了excel meta属性，原来的 row=true|false改为 orientation=landscape|l|row|r|portrait|p|column|c
</commit_message>
<xml_diff>
--- a/DesignerConfigs/Datas/common/全局常量配置表.xlsx
+++ b/DesignerConfigs/Datas/common/全局常量配置表.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\workspace\luban_examples\DesignerConfigs\Datas\common\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9542693-09B2-4354-9BCF-8F828FA022C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42BFE216-E679-4C32-AE65-84E90B44C193}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29760" yWindow="390" windowWidth="27645" windowHeight="14835" xr2:uid="{024915E7-E294-4FD7-9063-032AA423A689}"/>
+    <workbookView xWindow="35010" yWindow="3285" windowWidth="27645" windowHeight="14835" xr2:uid="{024915E7-E294-4FD7-9063-032AA423A689}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,11 +30,222 @@
     <t>##</t>
   </si>
   <si>
-    <t>row:false</t>
+    <t>通用参数名</t>
+  </si>
+  <si>
+    <t>程序中的字段名称</t>
+  </si>
+  <si>
+    <t>描述</t>
+  </si>
+  <si>
+    <t>具体参数</t>
+  </si>
+  <si>
+    <t>bag_capacity</t>
+  </si>
+  <si>
+    <t>背包容量</t>
+  </si>
+  <si>
+    <t>bag_capacity_special</t>
+  </si>
+  <si>
+    <t>额外添加的格子容量</t>
+  </si>
+  <si>
+    <t>bag_temp_expendable_capacity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  临时消耗品背包最大容量</t>
+  </si>
+  <si>
+    <t>bag_temp_tool_capacity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  临时工具背包每种工具类型的最大格子数量</t>
+  </si>
+  <si>
+    <t>bag_init_capacity</t>
+  </si>
+  <si>
+    <t>背包的初始容量</t>
+  </si>
+  <si>
+    <t>quick_bag_capacity</t>
+  </si>
+  <si>
+    <t>快捷背包的个数</t>
+  </si>
+  <si>
+    <t>cloth_bag_capacity</t>
+  </si>
+  <si>
+    <t>服装背包的最大容量</t>
+  </si>
+  <si>
+    <t>cloth_bag_init_capacity</t>
+  </si>
+  <si>
+    <t>服装背包的初始容量</t>
+  </si>
+  <si>
+    <t>cloth_bag_capacity_special</t>
+  </si>
+  <si>
+    <t>服装背包额外增加的格子容量</t>
+  </si>
+  <si>
+    <t>mail_box_capacity</t>
+  </si>
+  <si>
+    <t>玩家邮件最大容量</t>
+  </si>
+  <si>
+    <t>init_skills</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>初始技能</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>damage_param_c</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>damage_param_d</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>damage_param_e</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>damage_param_f</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>role_speed</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>角色速度</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>monster_speed</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>怪物速度</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>init_custom_collocation_num</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>自定义套装最大数量</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>init_suit_id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>初始套装id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>init_energy</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>玩家初始能量</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bag_init_items_drop_id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>背包初始内容</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>battle_total_time</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>换装比拼时间（进入战斗的计时时间）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cloth_jewery_num_max</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>首饰可穿戴的最大数量</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>初始体力数值</t>
+  </si>
+  <si>
+    <t>初始体力上限</t>
+  </si>
+  <si>
+    <t>init_viality</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>max_viality</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>体力回复速度（参数为每点所需时</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>per_viality_recovery_time</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>换装比拼能量上限</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>clothbattle_energy_max</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cloth_fast_change_cd</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>快捷换装CD时间</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>init_quest_id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">  角色初始任务id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>quest_guide_h</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>目标为坐标时的引导点距地面的高度</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <r>
-      <t>t</t>
+      <t>o</t>
     </r>
     <r>
       <rPr>
@@ -45,223 +256,13 @@
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
-      <t>itle_rows:2</t>
+      <t>rientation=portrait</t>
     </r>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>通用参数名</t>
-  </si>
-  <si>
-    <t>程序中的字段名称</t>
-  </si>
-  <si>
-    <t>描述</t>
-  </si>
-  <si>
-    <t>具体参数</t>
-  </si>
-  <si>
-    <t>bag_capacity</t>
-  </si>
-  <si>
-    <t>背包容量</t>
-  </si>
-  <si>
-    <t>bag_capacity_special</t>
-  </si>
-  <si>
-    <t>额外添加的格子容量</t>
-  </si>
-  <si>
-    <t>bag_temp_expendable_capacity</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  临时消耗品背包最大容量</t>
-  </si>
-  <si>
-    <t>bag_temp_tool_capacity</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  临时工具背包每种工具类型的最大格子数量</t>
-  </si>
-  <si>
-    <t>bag_init_capacity</t>
-  </si>
-  <si>
-    <t>背包的初始容量</t>
-  </si>
-  <si>
-    <t>quick_bag_capacity</t>
-  </si>
-  <si>
-    <t>快捷背包的个数</t>
-  </si>
-  <si>
-    <t>cloth_bag_capacity</t>
-  </si>
-  <si>
-    <t>服装背包的最大容量</t>
-  </si>
-  <si>
-    <t>cloth_bag_init_capacity</t>
-  </si>
-  <si>
-    <t>服装背包的初始容量</t>
-  </si>
-  <si>
-    <t>cloth_bag_capacity_special</t>
-  </si>
-  <si>
-    <t>服装背包额外增加的格子容量</t>
-  </si>
-  <si>
-    <t>mail_box_capacity</t>
-  </si>
-  <si>
-    <t>玩家邮件最大容量</t>
-  </si>
-  <si>
-    <t>init_skills</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>初始技能</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>damage_param_c</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>damage_param_d</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>damage_param_e</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>damage_param_f</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>role_speed</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>角色速度</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>monster_speed</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>怪物速度</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>init_custom_collocation_num</t>
+    <t>title_rows=2</t>
     <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>自定义套装最大数量</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>init_suit_id</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>初始套装id</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>init_energy</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>玩家初始能量</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>bag_init_items_drop_id</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>背包初始内容</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>battle_total_time</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>换装比拼时间（进入战斗的计时时间）</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>cloth_jewery_num_max</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>首饰可穿戴的最大数量</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>初始体力数值</t>
-  </si>
-  <si>
-    <t>初始体力上限</t>
-  </si>
-  <si>
-    <t>init_viality</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>max_viality</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>体力回复速度（参数为每点所需时</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>per_viality_recovery_time</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>换装比拼能量上限</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>clothbattle_energy_max</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>cloth_fast_change_cd</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>快捷换装CD时间</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>init_quest_id</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">  角色初始任务id</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>quest_guide_h</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>目标为坐标时的引导点距地面的高度</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -405,7 +406,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -438,11 +439,14 @@
     <xf numFmtId="0" fontId="7" fillId="6" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
-    <cellStyle name="好" xfId="1" builtinId="26"/>
     <cellStyle name="差" xfId="2" builtinId="27"/>
     <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="好" xfId="1" builtinId="26"/>
     <cellStyle name="适中" xfId="3" builtinId="28"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -758,7 +762,7 @@
   <dimension ref="A1:G42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -772,11 +776,11 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
+      <c r="B1" s="12" t="s">
+        <v>61</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>2</v>
+        <v>62</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -792,7 +796,7 @@
     </row>
     <row r="3" spans="1:7" ht="72.75" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B3" s="4"/>
       <c r="C3" s="5"/>
@@ -802,13 +806,13 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="6" t="s">
         <v>4</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>6</v>
       </c>
       <c r="D4" s="6"/>
       <c r="E4" s="6"/>
@@ -824,10 +828,10 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C6" s="6">
         <v>1101001101</v>
@@ -838,10 +842,10 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C7" s="6">
         <v>150</v>
@@ -860,10 +864,10 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="8" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C9" s="8">
         <v>500</v>
@@ -875,10 +879,10 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="8" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C10" s="8">
         <v>50</v>
@@ -890,10 +894,10 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="8" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C11" s="8">
         <v>10</v>
@@ -905,10 +909,10 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="8" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C12" s="8">
         <v>4</v>
@@ -920,10 +924,10 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C13" s="8">
         <v>100</v>
@@ -935,10 +939,10 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="8" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C14" s="8">
         <v>4</v>
@@ -950,10 +954,10 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="8" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C15" s="8">
         <v>1000</v>
@@ -965,10 +969,10 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="8" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C16" s="8">
         <v>500</v>
@@ -980,10 +984,10 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="8" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C17" s="8">
         <v>50</v>
@@ -995,10 +999,10 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="8" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C18" s="8">
         <v>1</v>
@@ -1018,10 +1022,10 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" s="10" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C20" s="10">
         <v>1002</v>
@@ -1032,10 +1036,10 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" s="10" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B21" s="10" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C21" s="10">
         <v>3</v>
@@ -1054,10 +1058,10 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" s="7" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C23" s="7">
         <v>100</v>
@@ -1076,10 +1080,10 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" s="11" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B25" s="11" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C25" s="11">
         <v>1001</v>
@@ -1090,7 +1094,7 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" s="11" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B26" s="11"/>
       <c r="C26" s="11">
@@ -1102,7 +1106,7 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" s="11" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B27" s="11"/>
       <c r="C27" s="11">
@@ -1114,7 +1118,7 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" s="11" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B28" s="11"/>
       <c r="C28" s="11">
@@ -1126,7 +1130,7 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" s="11" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B29" s="11"/>
       <c r="C29" s="11">
@@ -1146,10 +1150,10 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" s="8" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C31" s="8">
         <v>5</v>
@@ -1160,10 +1164,10 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" s="8" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B32" s="8" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C32" s="8">
         <v>5</v>
@@ -1174,10 +1178,10 @@
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" s="8" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B33" s="8" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C33" s="8">
         <v>0</v>
@@ -1188,10 +1192,10 @@
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" s="8" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B34" s="8" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C34" s="8">
         <v>4</v>
@@ -1202,10 +1206,10 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" s="8" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B35" s="8" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C35" s="8">
         <v>100</v>
@@ -1216,10 +1220,10 @@
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" s="8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B36" s="8" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C36" s="8">
         <v>100</v>
@@ -1230,10 +1234,10 @@
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" s="8" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B37" s="8" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C37" s="8">
         <v>300</v>
@@ -1260,10 +1264,10 @@
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" s="7" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B40" s="7" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C40" s="7">
         <v>40</v>
@@ -1274,10 +1278,10 @@
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" s="7" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B41" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C41" s="7">
         <v>5</v>
@@ -1288,10 +1292,10 @@
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" s="7" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B42" s="7" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C42" s="7">
         <v>1.5</v>

</xml_diff>

<commit_message>
更新luban-server, excel meta属性orientation不再支持 landscape|l|portrait|p这几个属性
</commit_message>
<xml_diff>
--- a/DesignerConfigs/Datas/common/全局常量配置表.xlsx
+++ b/DesignerConfigs/Datas/common/全局常量配置表.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\workspace\luban_examples\DesignerConfigs\Datas\common\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42BFE216-E679-4C32-AE65-84E90B44C193}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1979087A-24D8-47AD-91AA-6CBA97C3ACAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="35010" yWindow="3285" windowWidth="27645" windowHeight="14835" xr2:uid="{024915E7-E294-4FD7-9063-032AA423A689}"/>
+    <workbookView xWindow="570" yWindow="255" windowWidth="27645" windowHeight="14835" xr2:uid="{024915E7-E294-4FD7-9063-032AA423A689}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -244,24 +244,11 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <r>
-      <t>o</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>rientation=portrait</t>
-    </r>
+    <t>title_rows=2</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>title_rows=2</t>
+    <t>orientation=c</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -762,7 +749,7 @@
   <dimension ref="A1:G42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -777,10 +764,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>61</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>62</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>

</xml_diff>